<commit_message>
Drag and Drop feature
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/last.xlsx
+++ b/src/test/resources/testdata/last.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
   <si>
     <t>FirstName</t>
   </si>
@@ -27,43 +27,46 @@
     <t>Password</t>
   </si>
   <si>
-    <t>John</t>
+    <t>Johni</t>
   </si>
   <si>
     <t>Smith</t>
   </si>
   <si>
-    <t>john2022</t>
+    <t>JoshNeo5i</t>
+  </si>
+  <si>
+    <t>Secret@123i</t>
+  </si>
+  <si>
+    <t>Maryi</t>
+  </si>
+  <si>
+    <t>Anni</t>
+  </si>
+  <si>
+    <t>MarNeo5i</t>
+  </si>
+  <si>
+    <t>Davidi</t>
+  </si>
+  <si>
+    <t>Browni</t>
+  </si>
+  <si>
+    <t>DavNeo5i</t>
+  </si>
+  <si>
+    <t>Irma</t>
+  </si>
+  <si>
+    <t>Neotech</t>
+  </si>
+  <si>
+    <t>irmaNEO</t>
   </si>
   <si>
     <t>Secret@123</t>
-  </si>
-  <si>
-    <t>Mary</t>
-  </si>
-  <si>
-    <t>Ann</t>
-  </si>
-  <si>
-    <t>mary2022</t>
-  </si>
-  <si>
-    <t>David</t>
-  </si>
-  <si>
-    <t>Brown</t>
-  </si>
-  <si>
-    <t>david2022</t>
-  </si>
-  <si>
-    <t>Irma</t>
-  </si>
-  <si>
-    <t>Neotech</t>
-  </si>
-  <si>
-    <t>irmaNEO</t>
   </si>
 </sst>
 </file>
@@ -104,7 +107,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -127,13 +130,100 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -143,10 +233,37 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1202,7 +1319,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1212,8 +1329,7 @@
     <col min="2" max="2" width="23.8516" style="1" customWidth="1"/>
     <col min="3" max="3" width="25.3516" style="1" customWidth="1"/>
     <col min="4" max="4" width="28.8516" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.8516" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.8516" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.8516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="22" customHeight="1">
@@ -1229,7 +1345,6 @@
       <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="E1" s="3"/>
     </row>
     <row r="2" ht="22" customHeight="1">
       <c r="A2" t="s" s="2">
@@ -1244,7 +1359,6 @@
       <c r="D2" t="s" s="2">
         <v>7</v>
       </c>
-      <c r="E2" s="3"/>
     </row>
     <row r="3" ht="22" customHeight="1">
       <c r="A3" t="s" s="2">
@@ -1259,7 +1373,6 @@
       <c r="D3" t="s" s="2">
         <v>7</v>
       </c>
-      <c r="E3" s="3"/>
     </row>
     <row r="4" ht="22" customHeight="1">
       <c r="A4" t="s" s="2">
@@ -1274,49 +1387,6 @@
       <c r="D4" t="s" s="2">
         <v>7</v>
       </c>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" ht="15.35" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" ht="15.35" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" ht="15.35" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" ht="15.35" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" ht="15.35" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" ht="15.35" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1329,14 +1399,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1667" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="11.1719" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="11.1719" style="4" customWidth="1"/>
+    <col min="1" max="5" width="11.1719" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="11.1719" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.35" customHeight="1">
@@ -1352,7 +1422,7 @@
       <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="E1" s="3"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" ht="15.35" customHeight="1">
       <c r="A2" t="s" s="2">
@@ -1365,9 +1435,65 @@
         <v>16</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="E2" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" ht="15.35" customHeight="1">
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" ht="15.35" customHeight="1">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="10"/>
+    </row>
+    <row r="5" ht="15.35" customHeight="1">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10"/>
+    </row>
+    <row r="6" ht="15.35" customHeight="1">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="10"/>
+    </row>
+    <row r="7" ht="15.35" customHeight="1">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10"/>
+    </row>
+    <row r="8" ht="15.35" customHeight="1">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10"/>
+    </row>
+    <row r="9" ht="15.35" customHeight="1">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" ht="15.35" customHeight="1">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1386,79 +1512,79 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1667" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="11.1719" style="5" customWidth="1"/>
-    <col min="6" max="16384" width="11.1719" style="5" customWidth="1"/>
+    <col min="1" max="5" width="11.1719" style="14" customWidth="1"/>
+    <col min="6" max="16384" width="11.1719" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.35" customHeight="1">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" ht="15.35" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" ht="15.35" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" ht="15.35" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" ht="15.35" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" ht="15.35" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" ht="15.35" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" ht="15.35" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" ht="15.35" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" ht="15.35" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>